<commit_message>
added Tv as a parameter
</commit_message>
<xml_diff>
--- a/atp/dll/gfm_gfl_ibr2/PVMOD_CodeBased_GFD_IBR_Average_Model 2 1.xlsx
+++ b/atp/dll/gfm_gfl_ibr2/PVMOD_CodeBased_GFD_IBR_Average_Model 2 1.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\emthubsupport\atp\dll\gfm_gfl_ibr2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB09C85-FAD7-49F3-B5A0-FCD528DFD55A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C987C7-AC83-49E9-9D91-F1656EDE6F86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="380" windowWidth="18670" windowHeight="19260" activeTab="1" xr2:uid="{C6E1BEA0-2B9B-4DF7-BE60-E98356452841}"/>
+    <workbookView xWindow="8610" yWindow="1430" windowWidth="27370" windowHeight="19260" activeTab="1" xr2:uid="{C6E1BEA0-2B9B-4DF7-BE60-E98356452841}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="109">
   <si>
     <t>The location of the model's DLL (example ..\test.dll) (DLLFile)</t>
   </si>
@@ -304,6 +305,66 @@
   </si>
   <si>
     <t>corrected from 0</t>
+  </si>
+  <si>
+    <t>PVMOD</t>
+  </si>
+  <si>
+    <t>fs - PWM switching frequency</t>
+  </si>
+  <si>
+    <t>Cf - LC filter capacitance (delta)</t>
+  </si>
+  <si>
+    <t>Rd - LC filter (series) damping resistance</t>
+  </si>
+  <si>
+    <t>Cdc - DC link capacitance</t>
+  </si>
+  <si>
+    <t>rad/pu/s</t>
+  </si>
+  <si>
+    <t>rad/pu/s2</t>
+  </si>
+  <si>
+    <t>pu/pu</t>
+  </si>
+  <si>
+    <t>pu/pu/s</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>says 1 in table 2-ii, 0 in table 2-vi</t>
+  </si>
+  <si>
+    <t>Vlvrt=0.9</t>
+  </si>
+  <si>
+    <t>Vhvrt=1.1</t>
+  </si>
+  <si>
+    <t>Tv - time constant filtering the d1 axis voltage in voltage control loop</t>
+  </si>
+  <si>
+    <t>-0.2 in table 2-ix but 0 in figure 2-17</t>
+  </si>
+  <si>
+    <t>doc says set KQV2=0 to disable</t>
+  </si>
+  <si>
+    <t>called DelI_flg, set 1 for IEEE 2800-2022</t>
+  </si>
+  <si>
+    <t>not provided in the DLL code</t>
+  </si>
+  <si>
+    <t>ipri_flg: 1 for reactive current priority, 0 for active current priority</t>
+  </si>
+  <si>
+    <t>added as a parameter 8/25/2025</t>
   </si>
 </sst>
 </file>
@@ -793,18 +854,21 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1596,10 +1660,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC310360-2ACA-444D-9621-73F8FD8E51EB}">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1609,639 +1673,802 @@
     <col min="3" max="3" width="13.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B1">
         <v>1388815360</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F1" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="F2" s="7">
+        <v>3060</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
         <v>600</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>600</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="F4">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>1000000</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>1000000</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="F5">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B6" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C6" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="F6" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B8" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C8" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="F8" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" s="4">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="F10" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>25.4</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>25.4</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="F12">
+        <v>40</v>
+      </c>
+      <c r="G12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>324</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>324</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="G13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>70</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>70</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="F14">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>376.99111799999997</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <v>376.99111799999997</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>1.9</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>1.9</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <v>1200</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <v>1200</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="F17">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>15</v>
       </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>16</v>
       </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>17</v>
       </c>
-      <c r="B19">
+      <c r="B20">
         <v>0.56000000000000005</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="B20">
+      <c r="B21">
         <v>5.18</v>
       </c>
-      <c r="C20">
+      <c r="C21">
         <v>5.18</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="F21">
+        <v>5.18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>19</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>52.91</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <v>52.91</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="F22">
+        <v>52.91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>20</v>
       </c>
-      <c r="B22">
+      <c r="B23">
         <v>0.1</v>
       </c>
-      <c r="C22">
+      <c r="C23">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="F23">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>21</v>
       </c>
-      <c r="B23">
+      <c r="B24">
         <v>-5.9999999999999995E-4</v>
       </c>
-      <c r="C23">
+      <c r="C24">
         <v>-5.9999999999999995E-4</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="F24">
+        <v>-5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>22</v>
       </c>
-      <c r="B24">
+      <c r="B25">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="C24">
+      <c r="C25">
         <v>5.9999999999999995E-4</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="F25">
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>23</v>
       </c>
-      <c r="B25">
+      <c r="B26">
         <v>20</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C26" s="3">
         <v>20</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D26" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="F26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>24</v>
       </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="C26" s="3">
-        <v>0</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0</v>
+      </c>
+      <c r="D27" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="F27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>25</v>
       </c>
-      <c r="B27">
+      <c r="B28">
         <v>1E-3</v>
       </c>
-      <c r="C27">
+      <c r="C28">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>26</v>
       </c>
-      <c r="B28">
-        <v>0</v>
-      </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>27</v>
       </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29" s="5">
-        <v>0</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0</v>
+      </c>
+      <c r="D30" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>28</v>
       </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
-      <c r="C30" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>29</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C32">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+      <c r="F32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>30</v>
       </c>
-      <c r="B32">
+      <c r="B33">
         <v>1.01</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C33" s="3">
         <v>1.01</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+      <c r="F33">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>31</v>
       </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
-      <c r="C33" s="3">
-        <v>0</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34" s="3">
+        <v>0</v>
+      </c>
+      <c r="D34" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+      <c r="F34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>32</v>
       </c>
-      <c r="B34">
+      <c r="B35">
         <v>100</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C35" s="3">
         <v>100</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D35" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+      <c r="F35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>33</v>
       </c>
-      <c r="B35">
+      <c r="B36">
         <v>-0.4</v>
       </c>
-      <c r="C35">
+      <c r="C36">
         <v>-0.4</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+      <c r="F36">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>34</v>
       </c>
-      <c r="B36">
+      <c r="B37">
         <v>0.4</v>
       </c>
-      <c r="C36">
+      <c r="C37">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+      <c r="F37">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>35</v>
       </c>
-      <c r="B37">
-        <v>0</v>
-      </c>
-      <c r="C37" s="3">
-        <v>0</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38" s="3">
+        <v>0</v>
+      </c>
+      <c r="D38" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+      <c r="F38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>36</v>
       </c>
-      <c r="B38">
+      <c r="B39">
         <v>40</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C39" s="3">
         <v>40</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+      <c r="F39">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>37</v>
       </c>
-      <c r="B39">
+      <c r="B40">
         <v>-0.1</v>
       </c>
-      <c r="C39">
+      <c r="C40">
         <v>-0.1</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+      <c r="F40">
+        <v>-0.1</v>
+      </c>
+      <c r="G40" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>38</v>
       </c>
-      <c r="B40">
+      <c r="B41">
         <v>0.1</v>
       </c>
-      <c r="C40">
+      <c r="C41">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+      <c r="F41">
+        <v>0.1</v>
+      </c>
+      <c r="G41" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>39</v>
       </c>
-      <c r="B41">
+      <c r="B42">
         <v>2</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C42" s="3">
         <v>2</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D42" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+      <c r="F42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>40</v>
       </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42" s="8">
-        <v>1</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" s="6">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+      <c r="F43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>41</v>
       </c>
-      <c r="B43">
-        <v>0</v>
-      </c>
-      <c r="C43" s="3">
-        <v>0</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44" s="3">
+        <v>0</v>
+      </c>
+      <c r="D44" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+      <c r="F44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>42</v>
       </c>
-      <c r="B44">
+      <c r="B45">
         <v>-0.1</v>
       </c>
-      <c r="C44">
+      <c r="C45">
         <v>-0.1</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>43</v>
       </c>
-      <c r="B45">
+      <c r="B46">
         <v>0.1</v>
       </c>
-      <c r="C45">
+      <c r="C46">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+      <c r="F46">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>44</v>
       </c>
-      <c r="B46">
+      <c r="B47">
         <v>2</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C47" s="3">
         <v>2</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D47" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
+      <c r="F47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>45</v>
       </c>
-      <c r="B47">
-        <v>0</v>
-      </c>
-      <c r="C47" s="8">
-        <v>0</v>
-      </c>
-      <c r="D47" t="s">
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48" s="6">
+        <v>0</v>
+      </c>
+      <c r="D48" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
+      <c r="F48" t="s">
+        <v>98</v>
+      </c>
+      <c r="G48" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>46</v>
       </c>
-      <c r="B48">
-        <v>1</v>
-      </c>
-      <c r="C48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>47</v>
       </c>
-      <c r="B49">
+      <c r="B50">
         <v>0.32324999999999998</v>
       </c>
-      <c r="C49">
+      <c r="C50">
         <v>0.32324999999999998</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
+      <c r="F50">
+        <v>0.9</v>
+      </c>
+      <c r="G50" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>48</v>
       </c>
-      <c r="B50">
+      <c r="B51">
         <v>324</v>
       </c>
-      <c r="C50">
+      <c r="C51">
         <v>324</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
+      <c r="F51">
+        <v>900</v>
+      </c>
+      <c r="G51" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>49</v>
       </c>
-      <c r="B51">
+      <c r="B52">
         <v>99999</v>
       </c>
-      <c r="C51">
+      <c r="C52">
         <v>99999</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
+      <c r="F52">
+        <v>99999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>50</v>
       </c>
-      <c r="B52">
+      <c r="B53">
         <v>-99999</v>
       </c>
-      <c r="C52">
+      <c r="C53">
         <v>-99999</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
+      <c r="F53">
+        <v>-99999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>102</v>
+      </c>
+      <c r="C54">
+        <v>0.01</v>
+      </c>
+      <c r="F54">
+        <v>0.01</v>
+      </c>
+      <c r="G54" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
         <v>51</v>
-      </c>
-      <c r="B53">
-        <v>1E-4</v>
-      </c>
-      <c r="C53">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>52</v>
-      </c>
-      <c r="B54">
-        <v>0</v>
-      </c>
-      <c r="C54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>53</v>
       </c>
       <c r="B55">
         <v>1E-4</v>
@@ -2249,97 +2476,128 @@
       <c r="C55">
         <v>1E-4</v>
       </c>
-      <c r="D55" t="s">
+      <c r="F55">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>52</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>53</v>
+      </c>
+      <c r="B57">
+        <v>1E-4</v>
+      </c>
+      <c r="C57">
+        <v>1E-4</v>
+      </c>
+      <c r="D57" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56" s="7" t="s">
+      <c r="F57">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A58" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C56" s="7">
+      <c r="C58" s="5">
         <v>7.5000000000000002E-4</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D58" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
+      <c r="F58">
+        <v>7.5000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>93</v>
+      </c>
+      <c r="C59" s="5"/>
+      <c r="F59">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>91</v>
+      </c>
+      <c r="C60" s="5"/>
+      <c r="F60">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>92</v>
+      </c>
+      <c r="C61" s="5"/>
+      <c r="F61">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>107</v>
+      </c>
+      <c r="C62" s="5"/>
+      <c r="F62">
+        <v>1</v>
+      </c>
+      <c r="G62" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
         <v>54</v>
       </c>
-      <c r="B57">
-        <v>1</v>
-      </c>
-      <c r="C57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="F63">
+        <v>1</v>
+      </c>
+      <c r="G63" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
         <v>55</v>
       </c>
-      <c r="B58">
+      <c r="B64">
         <v>0.01</v>
       </c>
-      <c r="C58" s="7">
+      <c r="C64" s="5">
         <v>0.01</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D64" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>56</v>
-      </c>
-      <c r="B59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>57</v>
-      </c>
-      <c r="B60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>58</v>
-      </c>
-      <c r="B61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>59</v>
-      </c>
-      <c r="B62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>60</v>
-      </c>
-      <c r="B63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>61</v>
-      </c>
-      <c r="B64">
-        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -2347,7 +2605,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -2355,7 +2613,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -2363,7 +2621,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -2371,7 +2629,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -2379,7 +2637,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B70">
         <v>0</v>
@@ -2387,9 +2645,57 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
+        <v>62</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>63</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>64</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>65</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>66</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>67</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
         <v>68</v>
       </c>
-      <c r="B71">
+      <c r="B77">
         <v>0</v>
       </c>
     </row>

</xml_diff>